<commit_message>
Dagbokar uppfaersla arni vidir meistara djofull
</commit_message>
<xml_diff>
--- a/Dagbaekur/Árni/DagbokAr.xlsx
+++ b/Dagbaekur/Árni/DagbokAr.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="20730" windowHeight="11055"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -96,8 +96,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,6 +251,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -285,6 +286,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -460,19 +462,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -486,7 +488,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -512,7 +514,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C5" s="1">
         <v>41659</v>
       </c>
@@ -535,28 +537,34 @@
         <v>41665</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
+      <c r="D6">
+        <v>60</v>
+      </c>
       <c r="E6">
         <v>120</v>
       </c>
       <c r="J6">
         <f>SUM(C6:I6)</f>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>1</v>
       </c>
+      <c r="F7">
+        <v>120</v>
+      </c>
       <c r="J7">
         <f t="shared" ref="J7:J11" si="0">SUM(C7:I7)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>2</v>
       </c>
@@ -565,16 +573,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>4</v>
       </c>
+      <c r="G9">
+        <v>60</v>
+      </c>
       <c r="J9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>5</v>
       </c>
@@ -583,7 +594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
@@ -599,16 +610,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J12">
         <f>SUM(J6:J11)</f>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>16</v>
       </c>
@@ -634,7 +645,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:10">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C15" s="1">
         <v>41301</v>
       </c>
@@ -657,19 +668,16 @@
         <v>41307</v>
       </c>
     </row>
-    <row r="16" spans="2:10">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>3</v>
       </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
       <c r="J16">
         <f>SUM(C16:I16)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:10">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>1</v>
       </c>
@@ -684,25 +692,40 @@
         <v>180</v>
       </c>
     </row>
-    <row r="18" spans="2:10">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>2</v>
       </c>
+      <c r="D18">
+        <v>60</v>
+      </c>
+      <c r="E18">
+        <v>30</v>
+      </c>
       <c r="J18">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>4</v>
       </c>
+      <c r="C19">
+        <v>60</v>
+      </c>
+      <c r="D19">
+        <v>120</v>
+      </c>
+      <c r="E19">
+        <v>120</v>
+      </c>
       <c r="J19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>5</v>
       </c>
@@ -711,7 +734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:10">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>6</v>
       </c>
@@ -727,16 +750,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:10">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J22">
         <f>SUM(J16:J21)</f>
-        <v>180</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>18</v>
       </c>
@@ -762,7 +785,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="2:10">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
         <v>41673</v>
       </c>
@@ -785,7 +808,7 @@
         <v>41679</v>
       </c>
     </row>
-    <row r="26" spans="2:10">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>3</v>
       </c>
@@ -794,7 +817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:10">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>1</v>
       </c>
@@ -803,7 +826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:10">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>2</v>
       </c>
@@ -815,7 +838,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="2:10">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>4</v>
       </c>
@@ -828,16 +851,19 @@
       <c r="E29">
         <v>300</v>
       </c>
+      <c r="I29">
+        <v>60</v>
+      </c>
       <c r="J29">
         <f t="shared" si="2"/>
-        <v>820</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>5</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>60</v>
       </c>
       <c r="J30">
@@ -845,7 +871,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="2:10">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>6</v>
       </c>
@@ -861,16 +887,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:10">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J32">
         <f>SUM(J26:J31)</f>
-        <v>940</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>19</v>
       </c>
@@ -896,7 +922,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="2:10">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C35" s="1">
         <v>41680</v>
       </c>
@@ -919,7 +945,7 @@
         <v>41686</v>
       </c>
     </row>
-    <row r="36" spans="2:10">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>3</v>
       </c>
@@ -928,7 +954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:10">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>1</v>
       </c>
@@ -937,7 +963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:10">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>2</v>
       </c>
@@ -946,30 +972,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:10">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>4</v>
       </c>
+      <c r="C39">
+        <v>60</v>
+      </c>
+      <c r="D39">
+        <v>120</v>
+      </c>
+      <c r="E39">
+        <v>120</v>
+      </c>
+      <c r="H39">
+        <v>60</v>
+      </c>
       <c r="J39">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>5</v>
       </c>
+      <c r="E40">
+        <v>120</v>
+      </c>
       <c r="J40">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
+      <c r="D41" s="2">
+        <v>120</v>
+      </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
@@ -977,19 +1020,19 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J42">
         <f>SUM(J36:J41)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>22</v>
       </c>
@@ -1015,7 +1058,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="2:10">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C45" s="1">
         <v>41687</v>
       </c>
@@ -1038,16 +1081,19 @@
         <v>41693</v>
       </c>
     </row>
-    <row r="46" spans="2:10">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>3</v>
       </c>
+      <c r="C46">
+        <v>60</v>
+      </c>
       <c r="J46">
         <f>SUM(C46:I46)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>1</v>
       </c>
@@ -1056,125 +1102,146 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:10">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>2</v>
       </c>
+      <c r="D48">
+        <v>30</v>
+      </c>
+      <c r="E48">
+        <v>60</v>
+      </c>
       <c r="J48">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="2:10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>4</v>
       </c>
+      <c r="D49">
+        <v>120</v>
+      </c>
+      <c r="E49">
+        <v>60</v>
+      </c>
       <c r="J49">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="2:10">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>5</v>
       </c>
+      <c r="D50">
+        <v>60</v>
+      </c>
       <c r="J50">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="2:10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
+      <c r="E51" s="2">
+        <v>60</v>
+      </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="2:10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J52">
         <f>SUM(J46:J51)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="2:10">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="2:10">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>3</v>
       </c>
       <c r="D56">
-        <f t="shared" ref="D56:D61" si="5">J6+J16+J26+J36</f>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="57" spans="2:10">
+        <f>J6+J16+J26+J36+J46</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>1</v>
       </c>
       <c r="D57">
-        <f t="shared" si="5"/>
-        <v>180</v>
-      </c>
-    </row>
-    <row r="58" spans="2:10">
+        <f>J7+J17+J27+J37+J47</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>2</v>
       </c>
       <c r="D58">
-        <f t="shared" si="5"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="59" spans="2:10">
+        <f>J8+J18+J28+J38+J48</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>4</v>
       </c>
       <c r="D59">
-        <f t="shared" si="5"/>
-        <v>820</v>
-      </c>
-    </row>
-    <row r="60" spans="2:10">
+        <f>J9+J19+J29+J39+J49</f>
+        <v>1780</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>5</v>
       </c>
       <c r="D60">
-        <f t="shared" si="5"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="61" spans="2:10">
+        <f>J10+J20+J30+J40+J50</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="2:10">
+        <f>J11+J21+J31+J41+J51</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D62" s="3">
         <f>SUM(D56:D61)</f>
-        <v>1240</v>
+        <v>2980</v>
+      </c>
+      <c r="F62">
+        <f>D62/60</f>
+        <v>49.666666666666664</v>
       </c>
     </row>
   </sheetData>
@@ -1187,24 +1254,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Veit ekki hvort ég er að uppfæra eitthvað
</commit_message>
<xml_diff>
--- a/Dagbaekur/Árni/DagbokAr.xlsx
+++ b/Dagbaekur/Árni/DagbokAr.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="20730" windowHeight="11055"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -96,8 +96,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,7 +251,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -286,7 +285,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -462,19 +460,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -488,7 +486,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -514,7 +512,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10">
       <c r="C5" s="1">
         <v>41659</v>
       </c>
@@ -537,22 +535,19 @@
         <v>41665</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10">
       <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="D6">
-        <v>60</v>
-      </c>
       <c r="E6">
         <v>120</v>
       </c>
       <c r="J6">
         <f>SUM(C6:I6)</f>
-        <v>180</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -564,7 +559,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10">
       <c r="B8" t="s">
         <v>2</v>
       </c>
@@ -573,7 +568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -585,7 +580,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10">
       <c r="B10" t="s">
         <v>5</v>
       </c>
@@ -594,7 +589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10">
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
@@ -610,16 +605,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10">
       <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J12">
         <f>SUM(J6:J11)</f>
-        <v>360</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
       <c r="B14" t="s">
         <v>16</v>
       </c>
@@ -645,7 +640,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10">
       <c r="C15" s="1">
         <v>41301</v>
       </c>
@@ -668,7 +663,7 @@
         <v>41307</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10">
       <c r="B16" t="s">
         <v>3</v>
       </c>
@@ -677,7 +672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10">
       <c r="B17" t="s">
         <v>1</v>
       </c>
@@ -692,7 +687,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10">
       <c r="B18" t="s">
         <v>2</v>
       </c>
@@ -707,7 +702,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10">
       <c r="B19" t="s">
         <v>4</v>
       </c>
@@ -725,7 +720,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10">
       <c r="B20" t="s">
         <v>5</v>
       </c>
@@ -734,7 +729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10">
       <c r="B21" s="2" t="s">
         <v>6</v>
       </c>
@@ -750,7 +745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10">
       <c r="B22" s="3" t="s">
         <v>14</v>
       </c>
@@ -759,7 +754,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10">
       <c r="B24" t="s">
         <v>18</v>
       </c>
@@ -785,7 +780,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10">
       <c r="C25" s="1">
         <v>41673</v>
       </c>
@@ -808,7 +803,7 @@
         <v>41679</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10">
       <c r="B26" t="s">
         <v>3</v>
       </c>
@@ -817,7 +812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10">
       <c r="B27" t="s">
         <v>1</v>
       </c>
@@ -826,7 +821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10">
       <c r="B28" t="s">
         <v>2</v>
       </c>
@@ -838,7 +833,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10">
       <c r="B29" t="s">
         <v>4</v>
       </c>
@@ -859,7 +854,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10">
       <c r="B30" t="s">
         <v>5</v>
       </c>
@@ -871,7 +866,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10">
       <c r="B31" s="2" t="s">
         <v>6</v>
       </c>
@@ -887,7 +882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10">
       <c r="B32" s="3" t="s">
         <v>14</v>
       </c>
@@ -896,7 +891,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10">
       <c r="B34" t="s">
         <v>19</v>
       </c>
@@ -922,7 +917,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10">
       <c r="C35" s="1">
         <v>41680</v>
       </c>
@@ -945,7 +940,7 @@
         <v>41686</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10">
       <c r="B36" t="s">
         <v>3</v>
       </c>
@@ -954,7 +949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10">
       <c r="B37" t="s">
         <v>1</v>
       </c>
@@ -963,7 +958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10">
       <c r="B38" t="s">
         <v>2</v>
       </c>
@@ -972,7 +967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10">
       <c r="B39" t="s">
         <v>4</v>
       </c>
@@ -993,7 +988,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10">
       <c r="B40" t="s">
         <v>5</v>
       </c>
@@ -1005,7 +1000,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10">
       <c r="B41" s="2" t="s">
         <v>6</v>
       </c>
@@ -1023,7 +1018,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:10">
       <c r="B42" s="3" t="s">
         <v>14</v>
       </c>
@@ -1032,7 +1027,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10">
       <c r="B44" t="s">
         <v>22</v>
       </c>
@@ -1058,7 +1053,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10">
       <c r="C45" s="1">
         <v>41687</v>
       </c>
@@ -1081,7 +1076,7 @@
         <v>41693</v>
       </c>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:10">
       <c r="B46" t="s">
         <v>3</v>
       </c>
@@ -1093,7 +1088,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:10">
       <c r="B47" t="s">
         <v>1</v>
       </c>
@@ -1102,7 +1097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:10">
       <c r="B48" t="s">
         <v>2</v>
       </c>
@@ -1117,7 +1112,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:10">
       <c r="B49" t="s">
         <v>4</v>
       </c>
@@ -1132,7 +1127,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:10">
       <c r="B50" t="s">
         <v>5</v>
       </c>
@@ -1144,7 +1139,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:10">
       <c r="B51" s="2" t="s">
         <v>6</v>
       </c>
@@ -1162,7 +1157,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:10">
       <c r="B52" s="3" t="s">
         <v>14</v>
       </c>
@@ -1171,77 +1166,77 @@
         <v>450</v>
       </c>
     </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:10">
       <c r="B54" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:10">
       <c r="B56" t="s">
         <v>3</v>
       </c>
       <c r="D56">
-        <f>J6+J16+J26+J36+J46</f>
-        <v>240</v>
-      </c>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D56:D61" si="5">J6+J16+J26+J36+J46</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10">
       <c r="B57" t="s">
         <v>1</v>
       </c>
       <c r="D57">
-        <f>J7+J17+J27+J37+J47</f>
+        <f t="shared" si="5"/>
         <v>300</v>
       </c>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:10">
       <c r="B58" t="s">
         <v>2</v>
       </c>
       <c r="D58">
-        <f>J8+J18+J28+J38+J48</f>
+        <f t="shared" si="5"/>
         <v>240</v>
       </c>
     </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:10">
       <c r="B59" t="s">
         <v>4</v>
       </c>
       <c r="D59">
-        <f>J9+J19+J29+J39+J49</f>
+        <f t="shared" si="5"/>
         <v>1780</v>
       </c>
     </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:10">
       <c r="B60" t="s">
         <v>5</v>
       </c>
       <c r="D60">
-        <f>J10+J20+J30+J40+J50</f>
+        <f t="shared" si="5"/>
         <v>240</v>
       </c>
     </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:10">
       <c r="B61" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2">
-        <f>J11+J21+J31+J41+J51</f>
+        <f t="shared" si="5"/>
         <v>180</v>
       </c>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:10">
       <c r="B62" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D62" s="3">
         <f>SUM(D56:D61)</f>
-        <v>2980</v>
+        <v>2920</v>
       </c>
       <c r="F62">
         <f>D62/60</f>
-        <v>49.666666666666664</v>
+        <v>48.666666666666664</v>
       </c>
     </row>
   </sheetData>
@@ -1254,24 +1249,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>